<commit_message>
Extract and stage pipeline and ORM
</commit_message>
<xml_diff>
--- a/references/aact codebook.xlsx
+++ b/references/aact codebook.xlsx
@@ -1272,10 +1272,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
       <selection activeCell="F2" sqref="F2:F48"/>
     </sheetView>
   </sheetViews>
@@ -1351,7 +1350,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="3" spans="1:10" ht="15.75" thickBot="1">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1377,7 +1376,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="4" spans="1:10" ht="15.75" thickBot="1">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1403,7 +1402,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="5" spans="1:10" ht="15.75" thickBot="1">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1485,7 +1484,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="8" spans="1:10" ht="15.75" thickBot="1">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1541,7 +1540,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="10" spans="1:10" ht="15.75" thickBot="1">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1567,7 +1566,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="11" spans="1:10" ht="15.75" thickBot="1">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1595,7 +1594,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="12" spans="1:10" ht="15.75" thickBot="1">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1623,7 +1622,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="13" spans="1:10" ht="15.75" thickBot="1">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1681,7 +1680,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="15" spans="1:10" ht="15.75" thickBot="1">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1707,7 +1706,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="16" spans="1:10" ht="15.75" thickBot="1">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1765,7 +1764,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="18" spans="1:10" ht="15.75" thickBot="1">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1791,7 +1790,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="19" spans="1:10" ht="15.75" thickBot="1">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1817,7 +1816,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="20" spans="1:10" ht="15.75" thickBot="1">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1843,7 +1842,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="21" spans="1:10" ht="15.75" thickBot="1">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1869,7 +1868,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="22" spans="1:10" ht="15.75" thickBot="1">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -1895,7 +1894,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="23" spans="1:10" ht="15.75" thickBot="1">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -1921,7 +1920,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="24" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="24" spans="1:10" ht="15.75" thickBot="1">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -1947,7 +1946,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="25" spans="1:10" ht="15.75" thickBot="1">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -1973,7 +1972,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="26" spans="1:10" ht="15.75" thickBot="1">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2059,7 +2058,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="29" spans="1:10" ht="15.75" thickBot="1">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2117,7 +2116,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="31" spans="1:10" ht="15.75" thickBot="1">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2143,7 +2142,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="32" spans="1:10" ht="15.75" thickBot="1">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2317,7 +2316,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="38" spans="1:10" ht="15.75" thickBot="1">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -2345,7 +2344,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="39" spans="1:10" ht="15.75" thickBot="1">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2433,7 +2432,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="42" spans="1:10" ht="15.75" thickBot="1">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2461,7 +2460,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="43" spans="1:10" ht="15.75" thickBot="1">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2487,7 +2486,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="44" spans="1:10" ht="15.75" thickBot="1">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -2513,7 +2512,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="45" spans="1:10" ht="15.75" thickBot="1">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -2539,7 +2538,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="46" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="46" spans="1:10" ht="15.75" thickBot="1">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -2565,7 +2564,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="47" spans="1:10" ht="15.75" thickBot="1">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -2621,7 +2620,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="49" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="49" spans="1:10" ht="15.75" thickBot="1">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -2647,7 +2646,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="50" spans="1:10" ht="15.75" thickBot="1">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -2673,7 +2672,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="51" spans="1:10" ht="15.75" thickBot="1">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -2699,7 +2698,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="52" spans="1:10" ht="15.75" thickBot="1">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -2727,7 +2726,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="53" spans="1:10" ht="15.75" thickBot="1">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -2753,7 +2752,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="54" spans="1:10" ht="15.75" thickBot="1">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -2779,7 +2778,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="55" spans="1:10" ht="15.75" thickBot="1">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -2803,7 +2802,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="56" spans="1:10" ht="15.75" thickBot="1">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -2827,7 +2826,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="57" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="57" spans="1:10" ht="15.75" thickBot="1">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -2851,7 +2850,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="58" spans="1:10" ht="15.75" thickBot="1">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -2875,7 +2874,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="59" spans="1:10" ht="15.75" thickBot="1">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -2899,7 +2898,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="60" spans="1:10" ht="15.75" thickBot="1">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -2925,7 +2924,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="61" spans="1:10" ht="15.75" hidden="1" thickBot="1">
+    <row r="61" spans="1:10" ht="15.75" thickBot="1">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -2996,13 +2995,7 @@
       <c r="J65" s="11"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J61">
-    <filterColumn colId="2">
-      <customFilters>
-        <customFilter operator="notEqual" val=" "/>
-      </customFilters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:J61"/>
   <sortState ref="A2:XFD159">
     <sortCondition ref="A2:A159"/>
   </sortState>

</xml_diff>